<commit_message>
Remove search by user test
</commit_message>
<xml_diff>
--- a/Evaluation/Testing/Blackbox Testing - Template.xlsx
+++ b/Evaluation/Testing/Blackbox Testing - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pop/Desktop/Learning/UOL/Year 2/CM2020 - Agile Software Projects/Agile_Software_Projects_Team_17/Evaluation/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D073DE75-309F-0848-A5DF-77518999C6AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396813EC-9A9D-EB4E-8DAA-4063D74D71F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26780" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26780" windowHeight="16420" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="16" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="107">
   <si>
     <t>Test
 Procedure
@@ -270,13 +270,7 @@
     <t>1b.3</t>
   </si>
   <si>
-    <t>Type the search keyword "admin" in input box</t>
-  </si>
-  <si>
     <t>Type the search keyword "basic" in input box</t>
-  </si>
-  <si>
-    <t>Return code snippet contributed by user 'admin'</t>
   </si>
   <si>
     <t xml:space="preserve">Return code snippet with tag "basic" . </t>
@@ -510,8 +504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -527,6 +519,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -920,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5193BF18-10FC-DC4A-9DCD-1158C44022C4}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -934,18 +928,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="10"/>
     </row>
@@ -956,10 +950,10 @@
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.15">
@@ -967,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -977,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4"/>
@@ -987,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4"/>
@@ -997,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1017,7 +1011,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
@@ -1027,7 +1021,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
@@ -1055,11 +1049,11 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1074,35 +1068,35 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -1111,10 +1105,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1134,22 +1128,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -1212,10 +1206,10 @@
         <v>7.4</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1235,13 +1229,13 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1282,16 +1276,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="15"/>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1299,13 +1293,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1313,13 +1307,13 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1327,13 +1321,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1341,13 +1335,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1358,10 +1352,10 @@
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1369,13 +1363,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1383,13 +1377,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28" x14ac:dyDescent="0.15">
@@ -1397,13 +1391,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1430,10 +1424,10 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="6" t="s">
         <v>58</v>
       </c>
@@ -1445,43 +1439,43 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="7" t="s">
         <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -1490,10 +1484,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1513,22 +1507,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -1594,7 +1588,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1604,10 +1598,10 @@
         <v>1.5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1617,7 +1611,7 @@
         <v>1.6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>28</v>
@@ -1630,10 +1624,10 @@
         <v>1.7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1646,22 +1640,22 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="23" spans="2:6" ht="42" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="6" t="s">
         <v>58</v>
       </c>
@@ -1673,10 +1667,10 @@
       <c r="B24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="21"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1685,31 +1679,31 @@
       </c>
     </row>
     <row r="25" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
     </row>
     <row r="28" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
@@ -1718,10 +1712,10 @@
       <c r="C28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="16"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1741,22 +1735,22 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="2:6" ht="28" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
@@ -1822,7 +1816,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1835,16 +1829,22 @@
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C23:D23"/>
@@ -1857,12 +1857,6 @@
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1892,10 +1886,10 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="6" t="s">
         <v>58</v>
       </c>
@@ -1907,10 +1901,10 @@
       <c r="B3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="7" t="s">
         <v>59</v>
       </c>
@@ -1919,31 +1913,31 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -1952,10 +1946,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1975,22 +1969,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -2056,13 +2050,13 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2103,10 +2097,10 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="6" t="s">
         <v>58</v>
       </c>
@@ -2130,31 +2124,31 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -2163,10 +2157,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2186,22 +2180,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -2293,13 +2287,13 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2324,10 +2318,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9F86EA-E5B8-A94A-8246-AE68F70B041D}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2341,10 +2335,10 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="6" t="s">
         <v>58</v>
       </c>
@@ -2364,35 +2358,35 @@
         <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -2401,10 +2395,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2424,22 +2418,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -2486,23 +2480,23 @@
     </row>
     <row r="15" spans="2:6" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="B15" s="4">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="2:6" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="B16" s="4">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>74</v>
@@ -2510,27 +2504,14 @@
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="B17" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B18" s="17" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2538,7 +2519,7 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B17:F17"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
@@ -2571,11 +2552,11 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2590,35 +2571,35 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -2627,10 +2608,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2650,22 +2631,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -2744,7 +2725,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -2770,13 +2751,13 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2817,11 +2798,11 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2840,31 +2821,31 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -2873,10 +2854,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2896,22 +2877,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -2964,7 +2945,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
@@ -2997,13 +2978,13 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3044,11 +3025,11 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3058,7 +3039,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
@@ -3067,31 +3048,31 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -3100,10 +3081,10 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -3123,22 +3104,22 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:6" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -3191,7 +3172,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
@@ -3201,10 +3182,10 @@
         <v>6.4</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
@@ -3224,13 +3205,13 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>